<commit_message>
Refactor delivery and pickup summary pages to include additional data columns and improve total calculations
- Updated `summary_pickup.php` to sort by courier name and added ID column.
- Modified `delivery.php` to calculate totals for pending and canceled deliveries, and display them in separate tables.
- Enhanced `pick_up.php` to show canceled deliveries for the current month with total calculations.
- Created new delete functionality for couriers in `kurir.php` to remove associated records from both `mst_kurir` and `mst_user`.
- Adjusted various total labels across summary tables for consistency.
</commit_message>
<xml_diff>
--- a/adm/export/Data Delivery.xlsx
+++ b/adm/export/Data Delivery.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>DATA DELIVERY</t>
   </si>
@@ -47,58 +47,37 @@
     <t>KETERANGAN</t>
   </si>
   <si>
-    <t>RATNA</t>
-  </si>
-  <si>
-    <t>ONKU</t>
-  </si>
-  <si>
-    <t>ANSA</t>
-  </si>
-  <si>
-    <t>SUKSES</t>
-  </si>
-  <si>
-    <t>YUSUF</t>
-  </si>
-  <si>
-    <t>C69Z</t>
-  </si>
-  <si>
-    <t>DEA</t>
+    <t>BRBURHANUDDIN</t>
+  </si>
+  <si>
+    <t>ADIT</t>
+  </si>
+  <si>
+    <t>MMFQ</t>
+  </si>
+  <si>
+    <t>PRSYNDIA</t>
   </si>
   <si>
     <t>PENDING</t>
   </si>
   <si>
-    <t>JNJOJON</t>
-  </si>
-  <si>
-    <t>ADEK</t>
-  </si>
-  <si>
-    <t>HNXP</t>
-  </si>
-  <si>
-    <t>ANGGIA</t>
-  </si>
-  <si>
-    <t>PROSES</t>
-  </si>
-  <si>
-    <t>ADMINISTRATOR</t>
-  </si>
-  <si>
-    <t>ZCQE</t>
-  </si>
-  <si>
-    <t>RAYMOND RIOS</t>
-  </si>
-  <si>
-    <t>Y9R6</t>
-  </si>
-  <si>
-    <t>NDA</t>
+    <t>SADAM</t>
+  </si>
+  <si>
+    <t>WJUF</t>
+  </si>
+  <si>
+    <t>HAHAHA</t>
+  </si>
+  <si>
+    <t>CKOR</t>
+  </si>
+  <si>
+    <t>UDIN</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
   </si>
   <si>
     <t>TOTAL:</t>
@@ -135,6 +114,9 @@
   </si>
   <si>
     <t>TABEL CANCEL HARI INI</t>
+  </si>
+  <si>
+    <t>TOTAL CANCEL:</t>
   </si>
 </sst>
 </file>
@@ -519,10 +501,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -533,8 +515,8 @@
     <col min="5" max="5" width="21.566" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="15.139" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="21.566" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.998" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="12.568" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="11.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="11.283" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="16.425" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -580,28 +562,28 @@
         <v>1</v>
       </c>
       <c r="C5" s="4">
-        <v>2179</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
         <v>10</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4">
-        <v>12000</v>
-      </c>
-      <c r="I5" s="4">
-        <v>1000</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -609,28 +591,28 @@
         <v>2</v>
       </c>
       <c r="C6" s="4">
-        <v>28</v>
+        <v>2190</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="4">
+        <v>120000</v>
+      </c>
+      <c r="I6" s="4">
+        <v>3200</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="4">
-        <v>15</v>
-      </c>
-      <c r="I6" s="4">
-        <v>10</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -638,213 +620,224 @@
         <v>3</v>
       </c>
       <c r="C7" s="4">
-        <v>1479</v>
+        <v>2192</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="4">
+        <v>90000</v>
+      </c>
+      <c r="I7" s="4">
+        <v>3000</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H8" s="2">
+        <v>210000</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1638</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="4">
+        <v>120000</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3200</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1637</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2178</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="I16" s="4">
+        <v>10</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="G17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="2">
+        <v>120000</v>
+      </c>
+      <c r="I17" s="2">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1639</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>9000</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="4">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2177</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="4">
-        <v>12000</v>
-      </c>
-      <c r="I9" s="4">
-        <v>2000</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="G10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="2">
-        <v>24015</v>
-      </c>
-      <c r="I10" s="2">
-        <v>12016.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="H23" s="4">
+        <v>90000</v>
+      </c>
+      <c r="I23" s="4">
+        <v>3000</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="G24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1627</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="4">
-        <v>15</v>
-      </c>
-      <c r="I17" s="4">
-        <v>10</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="G18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="2">
-        <v>15</v>
-      </c>
-      <c r="I18" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="B21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="B23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>37</v>
+      <c r="H24" s="2">
+        <v>90000</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B20:J20"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>